<commit_message>
Sesion hablitada - Logout funcionando
</commit_message>
<xml_diff>
--- a/website/static/asistencia/excel/asistenciaFicha.xlsx
+++ b/website/static/asistencia/excel/asistenciaFicha.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No vino</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No vino</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
agregando css a la pagina web de asistencia
</commit_message>
<xml_diff>
--- a/website/static/asistencia/excel/asistenciaFicha.xlsx
+++ b/website/static/asistencia/excel/asistenciaFicha.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,486 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LuisaRamirez</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>JessicaArcila</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ManuelaSotoMarin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>JoselynArangoBedoya</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ManuelNorenaGuevera</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DannaMolinaZapata</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>YuriJohanaVinascoFonseca</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>LauraAndreaTrujilloRestrepo</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>JulianaRioMartinez</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ValentinaRamirezCuesta</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>HaroldValenciaGonzales</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>GeraldinPalacioMunos</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>MichellyHurtadoJimenez</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DamaraGiraldoBolivar</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SaraAcevedoMarin</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>YuranyRojasPulgarin</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>JulianaQuinteroArboleda</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>DuvanEsneiderDiazMontoya</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>YeilyFunesOsorio</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CrisLauraPadilla</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MelanyMorales</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SofiaVeraMartina</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MarianaValenciaZapata</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>JuanCamiloVasqeuz</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SebastianMejiaVasquez</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SantiagoMejiaAcevedo</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>EadySantiagoLondono</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>SalomeSisquiarcoRios</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>JhonatanMontanaSolano</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>SantiagoParraOsorio</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>YenniferJimenezAguila</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SamuelYepesOsorio</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Arreglando error del submit de asistencia
</commit_message>
<xml_diff>
--- a/website/static/asistencia/excel/asistenciaFicha.xlsx
+++ b/website/static/asistencia/excel/asistenciaFicha.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DavidAndresNorenaGiraldo</t>
+          <t>DavidLondoño</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,130 +466,10 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LucasArboledaBedoya</t>
+          <t>CarlosRiaño</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SebastianSalasCuartas</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>JuanPabloRojasArismendy</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SimonLopezPelaez</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>MiguelAngelCastillaBallestas</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>JuanDavidRiveraCasallas</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>EmmanuelMunozZapata</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>JuanDavidRuizAlzate</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>OrlandoRobertoVilladiegoOtero</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
         <is>
           <t>No vino</t>
         </is>

</xml_diff>

<commit_message>
Alerta al eliminar usuario - estilos delete
</commit_message>
<xml_diff>
--- a/website/static/asistencia/excel/asistenciaFicha.xlsx
+++ b/website/static/asistencia/excel/asistenciaFicha.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DavidLondoño</t>
+          <t>DavidAndresNorenaGiraldo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,10 +466,130 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CarlosRiaño</t>
+          <t>LucasArboledaBedoya</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SebastianSalasCuartas</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>JuanPabloRojasArismendy</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SimonLopezPelaez</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MiguelAngelCastillaBallestas</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>JuanDavidRiveraCasallas</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>EmmanuelMunozZapata</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>JuanDavidRuizAlzate</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>OrlandoRobertoVilladiegoOtero</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>No vino</t>
         </is>

</xml_diff>

<commit_message>
Conexion a una base de datos remota y arreglando caracteres utf-8
</commit_message>
<xml_diff>
--- a/website/static/asistencia/excel/asistenciaFicha.xlsx
+++ b/website/static/asistencia/excel/asistenciaFicha.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DavidAndresNorenaGiraldo</t>
+          <t>DavidLondoño</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>No vino</t>
+          <t>Presente</t>
         </is>
       </c>
     </row>
@@ -466,12 +466,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LucasArboledaBedoya</t>
+          <t>CarlosRiaño</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>No vino</t>
+          <t>Presente</t>
         </is>
       </c>
     </row>
@@ -481,115 +481,10 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SebastianSalasCuartas</t>
+          <t>AndrésPerea</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>JuanPabloRojasArismendy</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SimonLopezPelaez</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>MiguelAngelCastillaBallestas</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>JuanDavidRiveraCasallas</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>EmmanuelMunozZapata</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>JuanDavidRuizAlzate</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>No vino</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>OrlandoRobertoVilladiegoOtero</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
         <is>
           <t>No vino</t>
         </is>

</xml_diff>

<commit_message>
Pagina web con base de datos remota
</commit_message>
<xml_diff>
--- a/website/static/asistencia/excel/asistenciaFicha.xlsx
+++ b/website/static/asistencia/excel/asistenciaFicha.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DavidLondoño</t>
+          <t>LucasArboledaBedoya</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CarlosRiaño</t>
+          <t>DavidAndresNoreñaGiraldo</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -481,12 +481,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AndrésPerea</t>
+          <t>SebastianSalasCuartas</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>No vino</t>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DanielGomezLeon</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SamuelYepesOsorio</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Presente</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Todo listo para usarse
</commit_message>
<xml_diff>
--- a/website/static/asistencia/excel/asistenciaFicha.xlsx
+++ b/website/static/asistencia/excel/asistenciaFicha.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No vino</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No vino</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No vino</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No vino</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LeydiMoralesRubiano</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>No vino</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Alertas para ficha y fecha funcionando
</commit_message>
<xml_diff>
--- a/website/static/asistencia/excel/asistenciaFicha.xlsx
+++ b/website/static/asistencia/excel/asistenciaFicha.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LucasArboledaBedoya</t>
+          <t>DavidAndresNorenaGiraldo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DavidAndresNoreñaGiraldo</t>
+          <t>LucasArboledaBedoya</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DanielGomezLeon</t>
+          <t>JuanPabloRojasArismendy</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SamuelYepesOsorio</t>
+          <t>SimonLopezPelaez</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -526,10 +526,550 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>LeydiMoralesRubiano</t>
+          <t>MiguelAngelCastillaBallestas</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>JuanDavidRiveraCasallas</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>EmmanuelMunozZapata</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>JuanDavidRuizAlzate</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>OrlandoRobertoVilladiegoOtero</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LuisaRamirez</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>JessicaArcila</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ManuelaSotoMarin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>JoselynArangoBedoya</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ManuelNorenaGuevera</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DannaMolinaZapata</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>YuriJohanaVinascoFonseca</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>LauraAndreaTrujilloRestrepo</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>JulianaRioMartinez</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ValentinaRamirezCuesta</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>HaroldValenciaGonzales</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>GeraldinPalacioMunos</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>MichellyHurtadoJimenez</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DamaraGiraldoBolivar</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SaraAcevedoMarin</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>YuranyRojasPulgarin</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>JulianaQuinteroArboleda</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>DuvanEsneiderDiazMontoya</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>YeilyFunesOsorio</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CrisLauraPadilla</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MelanyMorales</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SofiaVeraMartina</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MarianaValenciaZapata</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>JuanCamiloVasqeuz</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SebastianMejiaVasquez</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SantiagoMejiaAcevedo</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>EadySantiagoLondono</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>SalomeSisquiarcoRios</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>JhonatanMontanaSolano</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>SantiagoParraOsorio</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>YenniferJimenezAguila</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>No vino</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SamuelYepesOsorio</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
         <is>
           <t>No vino</t>
         </is>

</xml_diff>